<commit_message>
Grafica de datos treminado
</commit_message>
<xml_diff>
--- a/uploads/bak_Libro2.xlsx
+++ b/uploads/bak_Libro2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\paretoIA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USUARIO\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,6 +21,12 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
+    <t xml:space="preserve">Variable </t>
+  </si>
+  <si>
+    <t>Calificacion</t>
+  </si>
+  <si>
     <t>Prueba 1</t>
   </si>
   <si>
@@ -28,12 +34,6 @@
   </si>
   <si>
     <t>Prueba 3</t>
-  </si>
-  <si>
-    <t>Variable</t>
-  </si>
-  <si>
-    <t>Valor</t>
   </si>
 </sst>
 </file>
@@ -355,22 +355,22 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B1" t="s">
-        <v>4</v>
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B2" s="1">
         <v>100</v>
@@ -378,7 +378,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="1">
         <v>100</v>
@@ -386,7 +386,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1">
         <v>100</v>

</xml_diff>